<commit_message>
Added the exact bond calculation steps; fixed a bug in the interest rate save; demoed the lambda expressions to sort a list.
</commit_message>
<xml_diff>
--- a/doc/functional doc/calcule.xlsx
+++ b/doc/functional doc/calcule.xlsx
@@ -1,21 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\practica\sedinta 14-07-2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SRL\practica\David\work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D01FF6-2E8F-4413-9D35-87F04D05C40E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94465193-BEE6-48D1-ACD6-63220A612084}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="411" activeTab="2" xr2:uid="{0C88586D-8BE9-4B09-86AE-84A87132582F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{0C88586D-8BE9-4B09-86AE-84A87132582F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="MArket Data" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="bond price" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +27,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="70">
   <si>
     <t>Numar ani</t>
   </si>
@@ -86,6 +90,9 @@
     <t>Data ajustata</t>
   </si>
   <si>
+    <t>???</t>
+  </si>
+  <si>
     <t>?</t>
   </si>
   <si>
@@ -114,18 +121,145 @@
   </si>
   <si>
     <t>interpolare liniara</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>COSTY</t>
+  </si>
+  <si>
+    <t>Ccy1</t>
+  </si>
+  <si>
+    <t>Ccy2</t>
+  </si>
+  <si>
+    <t>EUR</t>
+  </si>
+  <si>
+    <t>RON</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>SPOT</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>1W</t>
+  </si>
+  <si>
+    <t>pips</t>
+  </si>
+  <si>
+    <t>Ccy</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Days</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t>Formula calcul dobanda</t>
+  </si>
+  <si>
+    <t>Principal (RON)</t>
+  </si>
+  <si>
+    <t>Perioda (ani)</t>
+  </si>
+  <si>
+    <t>Rata a dobanzii (% pe an)</t>
+  </si>
+  <si>
+    <t>Perioada (luni)</t>
+  </si>
+  <si>
+    <t>Perioada in zile (fata de astazi)</t>
+  </si>
+  <si>
+    <t>Astazi</t>
+  </si>
+  <si>
+    <t>Numar de zile in an</t>
+  </si>
+  <si>
+    <t>Data scadenta (data la acre primesc banii)</t>
+  </si>
+  <si>
+    <t>Dobanda (RON)</t>
+  </si>
+  <si>
+    <t>Suma primita la termen</t>
+  </si>
+  <si>
+    <t>Formula calcul valoare obligatiune</t>
+  </si>
+  <si>
+    <t>Data Inceput perioada</t>
+  </si>
+  <si>
+    <t>Data sfarsit perioada</t>
+  </si>
+  <si>
+    <t>Data scadenta (data la care primesc banii)</t>
+  </si>
+  <si>
+    <t>Etapa 1: determinarea valorii fluxurilor de bani</t>
+  </si>
+  <si>
+    <t>Etapa 2: determinarea valorii prezente a fluxurilor de bani</t>
+  </si>
+  <si>
+    <t>Data platii</t>
+  </si>
+  <si>
+    <t>Suma</t>
+  </si>
+  <si>
+    <t>Zero rate</t>
+  </si>
+  <si>
+    <t>este rata dobanzii interpolata pentru data 10/07/2021 din setul de date disponibile la 12/08/2020</t>
+  </si>
+  <si>
+    <t>este rata dobanzii interpolata pentru data 10/07/2022 din setul de date disponibile la 12/08/2020</t>
+  </si>
+  <si>
+    <t>Valoarea prezenta a fluxului de bani</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P bani astazi la o rata a dobanzii r% pentru t ani =&gt; P*(1+r) la puterea (numarul de perioade din an * numarul de ani)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P bani astazi la o rata a dobanzii r% pentru t ani =&gt; P*(1+r*t)</t>
+  </si>
+  <si>
+    <t>Valoarea prezenta</t>
+  </si>
+  <si>
+    <t>Etapa 3: determinarea pretului obligatiunii</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="#,##0.000000000"/>
     <numFmt numFmtId="165" formatCode="0.00000000"/>
-    <numFmt numFmtId="166" formatCode="0.00000%"/>
+    <numFmt numFmtId="173" formatCode="0.000000000000"/>
+    <numFmt numFmtId="177" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +285,7 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -158,15 +293,8 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -191,6 +319,36 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -201,11 +359,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -214,12 +371,22 @@
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -299,7 +466,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet3!$D$1</c:f>
+              <c:f>'MArket Data'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -332,37 +499,9 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="0"/>
-            <c:dispEq val="0"/>
-          </c:trendline>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet3!$C$2:$C$4</c:f>
+              <c:f>'MArket Data'!$C$2:$C$4</c:f>
               <c:numCache>
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="3"/>
@@ -380,7 +519,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$D$2:$D$4</c:f>
+              <c:f>'MArket Data'!$D$2:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1135,14 +1274,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
+      <xdr:colOff>295275</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>144780</xdr:rowOff>
+      <xdr:rowOff>157162</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>129539</xdr:colOff>
-      <xdr:row>27</xdr:row>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>28576</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1471,7 +1610,7 @@
   <dimension ref="A3:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1530,7 +1669,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1911,18 +2050,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07ACE59F-5A56-40C1-AC09-FEF84E108B3D}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.44140625" customWidth="1"/>
     <col min="3" max="3" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
@@ -1938,6 +2077,9 @@
       <c r="D1" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="E1" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -1953,6 +2095,9 @@
       <c r="D2" s="5">
         <v>1E-3</v>
       </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
@@ -1968,6 +2113,9 @@
       <c r="D3" s="5">
         <v>2E-3</v>
       </c>
+      <c r="E3" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
@@ -1983,189 +2131,627 @@
       <c r="D4" s="5">
         <v>1.7000000000000001E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B5" s="6">
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B7" s="6">
         <v>44081</v>
       </c>
-      <c r="C5" s="6">
-        <v>44081</v>
-      </c>
-      <c r="D5" s="9">
-        <f>D9</f>
-        <v>1.3934426229508198E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B6" s="6">
+      <c r="D7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B8" s="6">
         <v>44328</v>
       </c>
-      <c r="C6" s="6">
-        <v>44328</v>
-      </c>
-      <c r="D6" s="9">
-        <f>D10</f>
-        <v>1.3538461538461539E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C7" s="6"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="C8" s="6"/>
-      <c r="D8" s="9"/>
+      <c r="D8" s="8" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B9" s="6">
-        <v>44081</v>
-      </c>
-      <c r="D9" s="8">
-        <f>D2+(B9-C2)*(D3-D2)/(C3-C2)</f>
-        <v>1.3934426229508198E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B10" s="6">
-        <v>44328</v>
-      </c>
-      <c r="D10" s="8">
-        <f>D3+(B10-C3)*(D4-D3)/(C4-C3)</f>
-        <v>1.3538461538461539E-2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B11" s="6">
         <v>45155</v>
       </c>
-      <c r="D11" s="8">
-        <f>TREND(D2:D6,C2:C6,B11)</f>
-        <v>5.4762518857401243E-2</v>
+      <c r="D9" s="8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B12" s="6"/>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="B13" s="6">
-        <f>A33</f>
-        <v>44228</v>
-      </c>
-      <c r="D13" s="8">
-        <f>D9+(B13-B9)*(D10-D9)/(B10-B9)</f>
-        <v>8.6214498317770377E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A12" s="7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="6"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C30" s="2"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="B12" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="2" t="s">
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="B28" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>21</v>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29" s="6">
+        <v>44391</v>
+      </c>
+      <c r="B29">
+        <v>100</v>
+      </c>
+      <c r="C29" s="6">
+        <v>44029</v>
+      </c>
+      <c r="D29">
+        <f>A35</f>
+        <v>98.328416912487725</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32" s="6">
-        <v>44391</v>
-      </c>
-      <c r="B32">
-        <v>100</v>
-      </c>
-      <c r="C32" s="6">
-        <v>44029</v>
-      </c>
-      <c r="D32">
-        <f>B32/(1+B37)</f>
-        <v>98.328416912487725</v>
+      <c r="A32" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33" s="6">
-        <v>44228</v>
-      </c>
-      <c r="B33">
-        <v>100</v>
-      </c>
-      <c r="C33" s="6">
-        <v>44026</v>
-      </c>
-      <c r="D33">
-        <f>B32/(1+D13)</f>
-        <v>99.145224421589006</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="6"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="C35" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C36">
-        <f>A37*B37</f>
-        <v>1.6715845000000003</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37">
+      <c r="A33">
         <v>98.328500000000005</v>
       </c>
-      <c r="B37" s="5">
+      <c r="B33" s="5">
         <f>D4</f>
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="D37">
-        <f>A37+C36</f>
+      <c r="C33">
+        <f>A33*B33</f>
+        <v>1.6715845000000003</v>
+      </c>
+      <c r="D33">
+        <f>A33+C33</f>
         <v>100.0000845</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="7">
-        <f>D33</f>
-        <v>99.145224421589006</v>
-      </c>
-      <c r="B42" t="s">
-        <v>25</v>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f>B29/(1+B33)</f>
+        <v>98.328416912487725</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B38" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E934D0B-5FC2-4CB9-820F-F157E2F6712B}">
+  <dimension ref="A1:G9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="6">
+        <v>44029</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2">
+        <v>4.7567000000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="6">
+        <v>44029</v>
+      </c>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F3">
+        <v>256</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F4">
+        <f>F2+F3/10000</f>
+        <v>4.7823000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="6">
+        <v>44022</v>
+      </c>
+      <c r="B9" s="6">
+        <v>44387</v>
+      </c>
+      <c r="C9">
+        <f>B9-A9</f>
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC8F0F7C-ACD3-4EDE-B04C-000CFAE9E58B}">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" customWidth="1"/>
+    <col min="5" max="5" width="16.5546875" customWidth="1"/>
+    <col min="6" max="6" width="30.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.44140625" customWidth="1"/>
+    <col min="8" max="8" width="16.77734375" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B4" s="6">
+        <v>44055</v>
+      </c>
+      <c r="C4">
+        <v>100</v>
+      </c>
+      <c r="D4">
+        <v>6</v>
+      </c>
+      <c r="E4" s="6">
+        <v>44239</v>
+      </c>
+      <c r="F4">
+        <f>E4-B4</f>
+        <v>184</v>
+      </c>
+      <c r="G4">
+        <v>365</v>
+      </c>
+      <c r="H4" s="11">
+        <f>F4/G4</f>
+        <v>0.50410958904109593</v>
+      </c>
+      <c r="I4" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="J4">
+        <f>C4*I4*H4</f>
+        <v>2.0164383561643837</v>
+      </c>
+      <c r="K4">
+        <f>C4</f>
+        <v>100</v>
+      </c>
+      <c r="L4">
+        <f>K4+J4</f>
+        <v>102.01643835616439</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="9"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="L6">
+        <f>C4*POWER((1+I4),H4)</f>
+        <v>101.99682889922335</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B7" s="6"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="9"/>
+      <c r="L7">
+        <f>C4*(1+I4*H4)</f>
+        <v>102.01643835616439</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C11" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="M11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="N11" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C12" s="6">
+        <v>44055</v>
+      </c>
+      <c r="D12" s="6">
+        <v>44022</v>
+      </c>
+      <c r="E12" s="6">
+        <v>44387</v>
+      </c>
+      <c r="F12">
+        <v>100</v>
+      </c>
+      <c r="G12" s="15">
+        <v>44387</v>
+      </c>
+      <c r="H12" s="13">
+        <f>E12-D12</f>
+        <v>365</v>
+      </c>
+      <c r="I12">
+        <v>365</v>
+      </c>
+      <c r="J12" s="11">
+        <f>H12/I12</f>
+        <v>1</v>
+      </c>
+      <c r="K12" s="14">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="L12">
+        <f>F12*K12*J12</f>
+        <v>8.5</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12" s="16">
+        <f>M12+L12</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C13" s="6">
+        <v>44055</v>
+      </c>
+      <c r="D13" s="6">
+        <v>44387</v>
+      </c>
+      <c r="E13" s="6">
+        <v>44752</v>
+      </c>
+      <c r="F13">
+        <v>100</v>
+      </c>
+      <c r="G13" s="17">
+        <v>44752</v>
+      </c>
+      <c r="H13" s="13">
+        <f>E13-D13</f>
+        <v>365</v>
+      </c>
+      <c r="I13">
+        <v>365</v>
+      </c>
+      <c r="J13" s="11">
+        <f>H13/I13</f>
+        <v>1</v>
+      </c>
+      <c r="K13" s="14">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="L13">
+        <f>F13*K13*J13</f>
+        <v>8.5</v>
+      </c>
+      <c r="M13">
+        <v>100</v>
+      </c>
+      <c r="N13" s="18">
+        <f>M13+L13</f>
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B15" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C19" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C20" s="6">
+        <v>44055</v>
+      </c>
+      <c r="D20" s="15">
+        <v>44387</v>
+      </c>
+      <c r="E20">
+        <f>D20-C20</f>
+        <v>332</v>
+      </c>
+      <c r="F20">
+        <v>365</v>
+      </c>
+      <c r="G20">
+        <f>E20/F20</f>
+        <v>0.90958904109589045</v>
+      </c>
+      <c r="H20" s="16">
+        <v>8.5</v>
+      </c>
+      <c r="I20" t="s">
+        <v>63</v>
+      </c>
+      <c r="J20" s="5">
+        <v>1.6E-2</v>
+      </c>
+      <c r="K20">
+        <f>H20/(1+J20*G20)</f>
+        <v>8.378070383892501</v>
+      </c>
+      <c r="M20">
+        <f>K20*(1+J20*G20)</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C21" s="6">
+        <v>44055</v>
+      </c>
+      <c r="D21" s="17">
+        <v>44752</v>
+      </c>
+      <c r="E21">
+        <f>D21-C21</f>
+        <v>697</v>
+      </c>
+      <c r="F21">
+        <v>365</v>
+      </c>
+      <c r="G21">
+        <f>E21/F21</f>
+        <v>1.9095890410958904</v>
+      </c>
+      <c r="H21" s="18">
+        <v>108.5</v>
+      </c>
+      <c r="I21" t="s">
+        <v>64</v>
+      </c>
+      <c r="J21" s="5">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="K21">
+        <f>H21/(1+J21*G21)</f>
+        <v>104.89450292149832</v>
+      </c>
+      <c r="M21">
+        <f>K21*(1+J21*G21)</f>
+        <v>108.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>68</v>
+      </c>
+      <c r="K23">
+        <f>SUM(K20:K21)</f>
+        <v>113.27257330539082</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C26" s="20">
+        <f>K23/F12%</f>
+        <v>113.27257330539082</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>